<commit_message>
More modifications for camera ready
</commit_message>
<xml_diff>
--- a/paper/raw_data/revised/old_results/exp17_COMPARISON.xlsx
+++ b/paper/raw_data/revised/old_results/exp17_COMPARISON.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prodr\Documents\UCSD\MigrationResearch\MemPod\paper\raw_data\revised\old_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prodr\Documents\UCSD\MigrationResearch\MemPodCameraReady\paper\raw_data\revised\old_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4635" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="COMPARISON" sheetId="1" r:id="rId1"/>
@@ -3790,7 +3790,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'COMPARISON WITH HMA PENALTY'!$M$2</c15:sqref>
@@ -3819,7 +3819,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$3:$K$32</c15:sqref>
@@ -3923,7 +3923,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'COMPARISON WITH HMA PENALTY'!$M$3:$M$32</c15:sqref>
@@ -4039,7 +4039,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'COMPARISON WITH HMA PENALTY'!$P$2</c15:sqref>
@@ -4068,7 +4068,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$3:$K$32</c15:sqref>
@@ -4172,7 +4172,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'COMPARISON WITH HMA PENALTY'!$P$3:$P$32</c15:sqref>
@@ -4469,6 +4469,2850 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NLM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$K$3:$K$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>astar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bwaves</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>bzip</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>cactus</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dealII</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>gems</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>lbm</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>leslie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>omnetpp</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>soplex</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>sphinx</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>xalanc</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>zeusmp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$M$3:$M$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3C3C-4CB9-8CD5-B75896B4EA0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>THM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$K$3:$K$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>astar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bwaves</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>bzip</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>cactus</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dealII</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>gems</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>lbm</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>leslie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>omnetpp</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>soplex</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>sphinx</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>xalanc</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>zeusmp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$N$3:$N$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.89265347198926537</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.009866257399693</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.81125509959203257</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93965683439367653</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96344445874629936</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.77580225498699051</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.06509253350351</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0277554304102978</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.83728216173878989</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.67709213863060014</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.81464872944693567</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.65694330320460148</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.68931005110732535</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95397705298440127</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0128294036061027</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3C3C-4CB9-8CD5-B75896B4EA0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HMA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="98500"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$K$3:$K$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>astar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bwaves</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>bzip</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>cactus</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dealII</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>gems</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>lbm</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>leslie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>omnetpp</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>soplex</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>sphinx</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>xalanc</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>zeusmp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$O$3:$O$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.94154038351281366</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0360580181036574</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0445451136979271</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9671914361728855</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0695341551732189</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0188150161812237</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0991320272425755</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1088088726648273</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0366421904916674</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0921584416980896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99669741179792104</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.79351819005338986</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.91097276241021075</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0223766179304112</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0799808872412957</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3C3C-4CB9-8CD5-B75896B4EA0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CAMEO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$K$3:$K$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>astar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bwaves</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>bzip</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>cactus</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dealII</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>gems</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>lbm</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>leslie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>omnetpp</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>soplex</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>sphinx</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>xalanc</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>zeusmp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$R$3:$R$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.3985239852398523</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0462617846963385</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5131989440844731</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3439367649893965</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3734071309048785</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1465741543798789</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2603701340140396</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1423974255832663</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96201292343841793</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0701606086221471</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7455904334828101</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5998356614626132</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0566439522998297</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.062137424261957</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0624133148404993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-3C3C-4CB9-8CD5-B75896B4EA0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MEMPOD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$K$3:$K$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>astar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bwaves</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>bzip</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>cactus</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dealII</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>gems</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>lbm</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>leslie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>omnetpp</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>soplex</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>sphinx</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>xalanc</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>zeusmp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$Q$3:$Q$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.85105669238510573</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0602937952203464</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76673866090712739</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87449392712550611</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.85261938473419996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66955767562879442</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0046798553499254</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.73089300080450537</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.72332093205404346</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.59932375316990705</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.72735426008968596</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.58668857847165157</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6450170357751277</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8584504318679903</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.82957697642163664</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3C3C-4CB9-8CD5-B75896B4EA0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$S$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HBM2GHz</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$K$3:$K$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>astar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bwaves</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>bzip</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>cactus</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dealII</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>gems</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>lbm</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>leslie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>omnetpp</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>soplex</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>sphinx</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>xalanc</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>zeusmp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$S$3:$S$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.55216370345521637</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.74325805744354301</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76121910247180224</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76460381723539617</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8205689277899344</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59843885516045103</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.63943841735800888</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.42276749798873692</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.70648130017622868</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.70076077768385459</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.57518684603886383</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.53779786359901394</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.62819420783645652</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.78200335181126723</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.62465325936199723</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-3C3C-4CB9-8CD5-B75896B4EA0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="343808720"/>
+        <c:axId val="343809376"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$L$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>DDR41600</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:tint val="88500"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$3:$K$17</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>astar</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>bwaves</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>bzip</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>cactus</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>dealII</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>gcc</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>gems</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>lbm</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>leslie</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>libquantum</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>omnetpp</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>soplex</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>sphinx</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>xalanc</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>zeusmp</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$L$3:$L$17</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>1.2690372358269038</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.1865818899364173</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.1467482601391887</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2.0279545016387122</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1.1406873471489254</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.2142237640936688</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.2939800042544141</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1.6013676588897829</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>1.3469747405521835</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>1.6267962806424345</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1.2863976083707025</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>1.3019720624486442</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>1.2655451448040886</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>1.1945339693180355</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>1.1827323162274619</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-3C3C-4CB9-8CD5-B75896B4EA0D}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$P$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>MPOLD</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:tint val="30000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$3:$K$17</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>astar</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>bwaves</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>bzip</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>cactus</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>dealII</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>gcc</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>gems</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>lbm</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>leslie</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>libquantum</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>omnetpp</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>soplex</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>sphinx</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>xalanc</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>zeusmp</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$P$3:$P$17</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>0.85005031868500502</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.0784915588686692</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.76673866090712739</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.86601118180065551</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.85249066803964479</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.67085862966175203</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.0482875983833229</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.73370876910699911</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.72371255140003921</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.59890109890109888</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.72406576980568005</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.58627773212818401</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.64544293015332199</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.85857934768596111</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.86477115117891823</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-3C3C-4CB9-8CD5-B75896B4EA0D}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="343808720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="343809376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="343809376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="343808720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NLM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$3:$K$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$K$18:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>mix1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mix10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mix11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mix12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mix2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mix3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mix4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>mix5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>mix6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mix7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>mix8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>mix9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>AVG HG</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>AVG MIX</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>AVG ALL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'COMPARISON WITH HMA PENALTY'!$M$3:$M$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$M$18:$M$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BC64-4D02-96D3-EDDE2C621C17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>THM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$3:$K$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$K$18:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>mix1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mix10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mix11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mix12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mix2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mix3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mix4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>mix5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>mix6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mix7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>mix8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>mix9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>AVG HG</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>AVG MIX</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>AVG ALL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'COMPARISON WITH HMA PENALTY'!$N$3:$N$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$N$18:$N$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.96494785631517954</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85314960629921266</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92342235878043011</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89307330195023538</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.91707080504364691</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.86210418794688459</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.90529905561385104</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.87003693444136654</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8685762426284751</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94838967793558704</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.91984402079722716</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.94453545518371174</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.89428063841370808</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.90869431643625198</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.90021328072970663</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BC64-4D02-96D3-EDDE2C621C17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HMA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="98500"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$3:$K$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$K$18:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>mix1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mix10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mix11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mix12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mix2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mix3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mix4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>mix5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>mix6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mix7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>mix8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>mix9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>AVG HG</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>AVG MIX</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>AVG ALL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'COMPARISON WITH HMA PENALTY'!$O$3:$O$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$O$18:$O$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.0494176534725104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0191443055184097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0203865770220097</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97229293832884933</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99733713306719385</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99789659556033228</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94442236796778267</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.93145884212074859</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99248091286273532</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0377165869645844</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9907856245895551</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0303755155185468</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0232063696567448</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.99720961513385264</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0125061551993446</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-BC64-4D02-96D3-EDDE2C621C17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CAMEO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$3:$K$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$K$18:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>mix1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mix10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mix11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mix12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mix2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mix3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mix4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>mix5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>mix6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mix7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>mix8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>mix9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>AVG HG</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>AVG MIX</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>AVG ALL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'COMPARISON WITH HMA PENALTY'!$R$3:$R$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$R$18:$R$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.705677867902665</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0354330708661421</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1652091704088867</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2368863483523873</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4468962172647915</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8338440585631597</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9635362014690452</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5916435826408126</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7517551249648975</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1604320864172835</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2157712305025996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.135970044465247</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3845812200922665</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4661136712749616</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4181398211139489</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-BC64-4D02-96D3-EDDE2C621C17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MEMPOD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$3:$K$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$K$18:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>mix1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mix10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mix11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mix12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mix2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mix3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mix4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>mix5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>mix6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mix7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>mix8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>mix9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>AVG HG</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>AVG MIX</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>AVG ALL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'COMPARISON WITH HMA PENALTY'!$Q$3:$Q$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$Q$18:$Q$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.87949015063731162</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77165354330708669</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.82651855353344361</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82447881640887699</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82347235693501453</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.76847122914538646</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.83788037775445967</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.81024930747922441</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.76720022465599558</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8839767953590717</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.86395147313691523</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.87713550198923473</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.80880540989713201</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.83238095238095233</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.81850905810846153</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-BC64-4D02-96D3-EDDE2C621C17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$S$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HBM2GHz</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$3:$K$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$K$18:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>mix1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mix10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>mix11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mix12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>mix2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mix3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mix4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>mix5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>mix6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mix7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>mix8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>mix9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>AVG HG</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>AVG MIX</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>AVG ALL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'COMPARISON WITH HMA PENALTY'!$S$3:$S$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'COMPARISON WITH HMA PENALTY'!$S$18:$S$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.60457705677867901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59173228346456697</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62727487591585906</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.74226630800269</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61469447138700295</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6012938372488934</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64139559286463799</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.67497691597414589</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.64785172704296545</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.68053610722144431</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.67937608318890819</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.63538497542710037</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.69165305596148874</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65312852022529444</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.67579643070905293</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-BC64-4D02-96D3-EDDE2C621C17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="441627056"/>
+        <c:axId val="441638864"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$L$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>DDR41600</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:tint val="88500"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$3:$K$32</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$18:$K$32</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>mix1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>mix10</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>mix11</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>mix12</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>mix2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>mix3</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>mix4</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>mix5</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>mix6</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>mix7</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>mix8</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>mix9</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>AVG HG</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>AVG MIX</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>AVG ALL</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$L$3:$L$32</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$L$18:$L$32</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>1.4006373117033604</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.5157480314960632</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.3072559678562987</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.5063887020847344</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1.2841901066925314</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.477357848144365</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.4108079748163695</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1.5163896583564174</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>1.5195169896096603</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>1.2892578515703141</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1.3901646447140383</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>1.3047039550666979</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>1.3070288546949771</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>1.4051408090117765</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>1.3474115475076502</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-BC64-4D02-96D3-EDDE2C621C17}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$P$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>MPOLD</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:tint val="30000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$3:$K$32</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$K$18:$K$32</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>mix1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>mix10</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>mix11</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>mix12</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>mix2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>mix3</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>mix4</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>mix5</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>mix6</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>mix7</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>mix8</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>mix9</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>AVG HG</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>AVG MIX</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>AVG ALL</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$P$3:$P$32</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'COMPARISON WITH HMA PENALTY'!$P$18:$P$32</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>0.86703360370799532</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.75984251968503946</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.83431812810210337</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.82229320780094151</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.83001939864209495</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.75519237316990118</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.83342077649527813</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.80286241920590951</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.75315922493681553</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.876375275055011</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.82300693240901224</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.86941259068570098</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.81518095074357444</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.82369687660010227</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.81868608954418598</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-BC64-4D02-96D3-EDDE2C621C17}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="441627056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441638864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="441638864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441627056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
   <a:schemeClr val="dk1"/>
@@ -4497,6 +7341,60 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
   <a:schemeClr val="dk1"/>
   <cs:variation>
@@ -5529,6 +8427,1012 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -5569,15 +9473,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>423332</xdr:colOff>
+      <xdr:colOff>433915</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>4233</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>529165</xdr:colOff>
+      <xdr:colOff>539748</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>80433</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5593,6 +9497,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>457727</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>157690</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>566207</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>58208</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>484187</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>67733</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>608542</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>153458</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8723,7 +12687,7 @@
   <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>